<commit_message>
Sort column Dept in ascending order
</commit_message>
<xml_diff>
--- a/resources/student.xlsx
+++ b/resources/student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\FilterSortTableActivity\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0F8C41-B301-4795-AE9B-B5026BF4F087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F729D23D-40DB-4F29-81A7-FB8FA0FF1637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1032,64 +1032,64 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D2" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G2" s="6">
-        <f t="shared" ref="G2:G15" si="0">SUM(D2:F2)/3</f>
-        <v>18</v>
+        <f>SUM(D2:F2)/3</f>
+        <v>19.333333333333332</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>1018</v>
+        <v>1021</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D3" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E3" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="6">
-        <f t="shared" si="0"/>
-        <v>14.666666666666666</v>
+        <f>SUM(D3:F3)/3</f>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>1015</v>
+        <v>1023</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D4" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="4">
         <v>15</v>
@@ -1098,272 +1098,272 @@
         <v>18</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>SUM(D4:F4)/3</f>
+        <v>16.666666666666668</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>1020</v>
+        <v>1012</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E5" s="4">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="F5" s="4">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" si="0"/>
-        <v>3.6666666666666665</v>
+        <f>SUM(D5:F5)/3</f>
+        <v>16.666666666666668</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>1022</v>
+        <v>1014</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E6" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F6" s="4">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" s="6">
-        <f t="shared" si="0"/>
+        <f>SUM(D6:F6)/3</f>
         <v>16.666666666666668</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>1021</v>
+        <v>1013</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D7" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="4">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4">
         <v>19</v>
       </c>
-      <c r="F7" s="4">
-        <v>20</v>
-      </c>
       <c r="G7" s="6">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f>SUM(D7:F7)/3</f>
+        <v>15.333333333333334</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>1010</v>
+        <v>1017</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E8" s="4">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F8" s="4">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" si="0"/>
-        <v>19.333333333333332</v>
+        <f>SUM(D8:F8)/3</f>
+        <v>14.333333333333334</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D9" s="4">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E9" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F9" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" si="0"/>
-        <v>13.333333333333334</v>
+        <f>SUM(D9:F9)/3</f>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>1016</v>
+        <v>1011</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E10" s="4">
         <v>18</v>
       </c>
       <c r="F10" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" si="0"/>
+        <f>SUM(D10:F10)/3</f>
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>1012</v>
+        <v>1016</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D11" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E11" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F11" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" si="0"/>
-        <v>16.666666666666668</v>
+        <f>SUM(D11:F11)/3</f>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="4">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4">
         <v>15</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="4">
-        <v>14</v>
-      </c>
-      <c r="E12" s="4">
-        <v>13</v>
       </c>
       <c r="F12" s="4">
         <v>19</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="0"/>
-        <v>15.333333333333334</v>
+        <f>SUM(D12:F12)/3</f>
+        <v>14.666666666666666</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>1014</v>
+        <v>1020</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D13" s="4">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E13" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F13" s="4">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="0"/>
-        <v>16.666666666666668</v>
+        <f>SUM(D13:F13)/3</f>
+        <v>3.6666666666666665</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D14" s="4">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E14" s="4">
+        <v>13</v>
+      </c>
+      <c r="F14" s="4">
         <v>15</v>
       </c>
-      <c r="F14" s="4">
-        <v>18</v>
-      </c>
       <c r="G14" s="6">
-        <f t="shared" si="0"/>
-        <v>16.666666666666668</v>
+        <f>SUM(D14:F14)/3</f>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
-        <v>1017</v>
+        <v>1022</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D15" s="12">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E15" s="12">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F15" s="12">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G15" s="13">
-        <f t="shared" si="0"/>
-        <v>14.333333333333334</v>
+        <f>SUM(D15:F15)/3</f>
+        <v>16.666666666666668</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1712,6 +1712,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G15">
+    <sortCondition ref="C2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>